<commit_message>
Author    : Priyanka Chaudhary Description : Updated Development Plan for Sprint-2 Updated File: Development Plan.xlsx
</commit_message>
<xml_diff>
--- a/collaterals/Development Plan.xlsx
+++ b/collaterals/Development Plan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\priyankachoudhary\Desktop\Voice Technology\Amico\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\AMICO App\amico_app\trunk\collaterals\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1351C47E-6488-412C-AF2A-D33760797B2E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE3A027B-F837-43A3-AB2B-76D703D171EA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="788" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="788" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Priyanka" sheetId="14" r:id="rId1"/>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="67">
   <si>
     <t>Notes:</t>
   </si>
@@ -118,10 +118,6 @@
   </si>
   <si>
     <t>April</t>
-  </si>
-  <si>
-    <t>AMICO-12
-(AMICO-32-37) - 5.5h</t>
   </si>
   <si>
     <t>AMICO-11
@@ -134,22 +130,7 @@
 (AMICO-25, AMICO-26 ) 1.5h</t>
   </si>
   <si>
-    <t>AMICO-20(AMCO-83-89) - 5.5h</t>
-  </si>
-  <si>
-    <t>AMICO-14(AMICO-40-45)  -5h</t>
-  </si>
-  <si>
-    <t>AMICO-15(48-54) -5h</t>
-  </si>
-  <si>
-    <t>AMICO-16(AMICO-57-62) 5h</t>
-  </si>
-  <si>
     <t>AMICO-18-5.5h</t>
-  </si>
-  <si>
-    <t>Testing</t>
   </si>
   <si>
     <t>Alpha Testing</t>
@@ -230,46 +211,12 @@
 AMICO-18 - 2h</t>
   </si>
   <si>
-    <t>AMICO-22 1.5h</t>
-  </si>
-  <si>
     <t>AMICO-24-4.5h
 * AMICO-100
 * AMICO-101
 * AMICO-102</t>
   </si>
   <si>
-    <t>Create Test cases
-1h
-Testing
-* AMICO -11, 12, 19</t>
-  </si>
-  <si>
-    <t>Testing 
-* AMICO -11, 12, 19</t>
-  </si>
-  <si>
-    <t>Bug Fixing for Conversation</t>
-  </si>
-  <si>
-    <t>Creatw test case
-Testing
-AMICO-20, 14,15,16,17</t>
-  </si>
-  <si>
-    <t>Creatw test case
-Testing
-AMICO-20, 14,15,16,18</t>
-  </si>
-  <si>
-    <t>Creatw test case
-Testing
-AMICO-20, 14,15,16,19</t>
-  </si>
-  <si>
-    <t>App Testing</t>
-  </si>
-  <si>
     <t>SPRINT GOALS</t>
   </si>
   <si>
@@ -346,6 +293,65 @@
   </si>
   <si>
     <t>Final Deployment</t>
+  </si>
+  <si>
+    <t>AMICO-22 1.5h
+AMICO-24-4.5h
+* AMICO-100
+* AMICO-101
+* AMICO-102</t>
+  </si>
+  <si>
+    <t>*AMICO-24
+*Preparation for Session on conversational Design
+*Send collaterals for App publishing for review</t>
+  </si>
+  <si>
+    <t>*Intent Writing for sharing file
+*Session on Conversation Design
+*Feedback Incorporation</t>
+  </si>
+  <si>
+    <t>*Feedback Incorporation
+*Intent Writing to store individual information
+*Review of Intents</t>
+  </si>
+  <si>
+    <t>*Review of Intents
+*Feedback Incorporation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AMICO-11
+(AMICO-26-29) 4.5h
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AMICO-12
+(AMICO-32-37) - 5.5h
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AMICO-12
+(AMICO-32-37) - 5.5h
+</t>
+  </si>
+  <si>
+    <t>AMICO-11
+(AMICO-26-29) 4.5h
+AMICO-19(AMICO-74-80) - 5.5h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AMICO-20(AMCO-83-89) - 5.5h
+AMICO-14(AMICO-40-45)  -5h
+Deployment
+</t>
+  </si>
+  <si>
+    <t>AMICO-15(48-54) -5h
+AMICO-16(AMICO-57-62) 5h</t>
+  </si>
+  <si>
+    <t>Testing</t>
   </si>
 </sst>
 </file>
@@ -355,7 +361,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Trebuchet MS"/>
@@ -491,6 +497,29 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Trebuchet MS"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -782,7 +811,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="9">
       <alignment horizontal="center"/>
@@ -825,9 +854,6 @@
     <xf numFmtId="164" fontId="9" fillId="9" borderId="4" xfId="5" applyFill="1" applyBorder="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="6" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="9" borderId="12" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
@@ -839,11 +865,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="6" applyNumberFormat="1" applyFont="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2">
       <alignment horizontal="left" indent="3"/>
     </xf>
@@ -874,6 +906,12 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="6" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" xfId="6" applyNumberFormat="1" applyFont="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="16">
     <cellStyle name="40% - Accent1" xfId="1" builtinId="31" customBuiltin="1"/>
@@ -893,7 +931,12 @@
     <cellStyle name="Title" xfId="9" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="15" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <color rgb="FF747474"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF747474"/>
@@ -1271,10 +1314,10 @@
     <tabColor theme="4" tint="-0.249977111117893"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H168"/>
+  <dimension ref="A1:K168"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1283,25 +1326,26 @@
     <col min="2" max="2" width="18.25" customWidth="1"/>
     <col min="3" max="8" width="17.625" customWidth="1"/>
     <col min="9" max="9" width="2.5" customWidth="1"/>
+    <col min="10" max="10" width="12.625" customWidth="1"/>
     <col min="14" max="14" width="6.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:11" ht="54" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A1" s="2"/>
       <c r="B1" s="1">
         <f ca="1">YEAR(TODAY())</f>
         <v>2019</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="6" t="s">
         <v>1</v>
@@ -1331,7 +1375,7 @@
         <v>SUNDAY</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4">
         <f t="array" aca="1" ref="B3:H3" ca="1">Days+1+DATE(Calendar1Year,Calendar1MonthOption,1)-WEEKDAY(DATE(Calendar1Year,Calendar1MonthOption,1),WeekdayOption)</f>
         <v>43556</v>
@@ -1361,7 +1405,7 @@
         <v>43562</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
@@ -1370,7 +1414,7 @@
       <c r="G4" s="12"/>
       <c r="H4" s="13"/>
     </row>
-    <row r="5" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="4">
         <f t="array" aca="1" ref="B5:H5" ca="1">Days+8+DATE(Calendar1Year,Calendar1MonthOption,1)-WEEKDAY(DATE(Calendar1Year,Calendar1MonthOption,1),WeekdayOption)</f>
         <v>43563</v>
@@ -1400,26 +1444,30 @@
         <v>43569</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="72" x14ac:dyDescent="0.35">
       <c r="B6" s="11" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="D6" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="16"/>
-      <c r="H6" s="17"/>
-    </row>
-    <row r="7" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E6" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="F6" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="G6" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="16"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="26"/>
+    </row>
+    <row r="7" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="4">
         <f t="array" aca="1" ref="B7:H7" ca="1">Days+15+DATE(Calendar1Year,Calendar1MonthOption,1)-WEEKDAY(DATE(Calendar1Year,Calendar1MonthOption,1),WeekdayOption)</f>
         <v>43570</v>
@@ -1449,26 +1497,30 @@
         <v>43576</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="12"/>
-      <c r="H8" s="13"/>
-    </row>
-    <row r="9" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" s="39" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="4">
         <f t="array" aca="1" ref="B9:H9" ca="1">Days+22+DATE(Calendar1Year,Calendar1MonthOption,1)-WEEKDAY(DATE(Calendar1Year,Calendar1MonthOption,1),WeekdayOption)</f>
         <v>43577</v>
@@ -1498,26 +1550,26 @@
         <v>43583</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="11" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E10" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="11" t="s">
         <v>12</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>13</v>
       </c>
       <c r="G10" s="12"/>
       <c r="H10" s="13"/>
     </row>
-    <row r="11" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="4">
         <f t="array" aca="1" ref="B11:H11" ca="1">Days+29+DATE(Calendar1Year,Calendar1MonthOption,1)-WEEKDAY(DATE(Calendar1Year,Calendar1MonthOption,1),WeekdayOption)</f>
         <v>43584</v>
@@ -1547,20 +1599,16 @@
         <v>43590</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>18</v>
-      </c>
+    <row r="12" spans="1:11" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
       <c r="G12" s="12"/>
       <c r="H12" s="13"/>
     </row>
-    <row r="13" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="4">
         <f t="array" aca="1" ref="B13:C13" ca="1">Days+36+DATE(Calendar1Year,Calendar1MonthOption,1)-WEEKDAY(DATE(Calendar1Year,Calendar1MonthOption,1),WeekdayOption)</f>
         <v>43591</v>
@@ -1569,40 +1617,40 @@
         <f ca="1"/>
         <v>43592</v>
       </c>
-      <c r="D13" s="30" t="s">
+      <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30"/>
-      <c r="H13" s="30"/>
-    </row>
-    <row r="14" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="31"/>
+    </row>
+    <row r="14" spans="1:11" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="31"/>
-    </row>
-    <row r="15" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
+    </row>
+    <row r="15" spans="1:11" ht="54" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A15" s="2"/>
       <c r="B15" s="1">
         <f ca="1">YEAR(DATE(Calendar1Year,Calendar1MonthOption+1,1))</f>
         <v>2019</v>
       </c>
-      <c r="C15" s="27" t="str">
+      <c r="C15" s="28" t="str">
         <f ca="1">TEXT(DATE(Calendar1Year,Calendar1MonthOption+1,1),"mmmm")</f>
         <v>May</v>
       </c>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="6" t="str">
         <f ca="1">UPPER(TEXT(B17,"dddd"))</f>
@@ -1837,22 +1885,22 @@
         <f ca="1"/>
         <v>43620</v>
       </c>
-      <c r="D27" s="29" t="s">
+      <c r="D27" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="E27" s="29"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="29"/>
-      <c r="H27" s="29"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="30"/>
     </row>
     <row r="28" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="31"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
     </row>
     <row r="29" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A29" s="2"/>
@@ -1860,12 +1908,12 @@
         <f ca="1">YEAR(DATE(Calendar2Year,Calendar2MonthOption+1,1))</f>
         <v>2019</v>
       </c>
-      <c r="C29" s="27" t="str">
+      <c r="C29" s="28" t="str">
         <f ca="1">TEXT(DATE(Calendar2Year,Calendar2MonthOption+1,1),"mmmm")</f>
         <v>June</v>
       </c>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="28"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
@@ -2105,22 +2153,22 @@
         <f ca="1"/>
         <v>43648</v>
       </c>
-      <c r="D41" s="29" t="s">
+      <c r="D41" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="E41" s="29"/>
-      <c r="F41" s="29"/>
-      <c r="G41" s="29"/>
-      <c r="H41" s="29"/>
+      <c r="E41" s="30"/>
+      <c r="F41" s="30"/>
+      <c r="G41" s="30"/>
+      <c r="H41" s="30"/>
     </row>
     <row r="42" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="8"/>
       <c r="C42" s="8"/>
-      <c r="D42" s="31"/>
-      <c r="E42" s="31"/>
-      <c r="F42" s="31"/>
-      <c r="G42" s="31"/>
-      <c r="H42" s="31"/>
+      <c r="D42" s="32"/>
+      <c r="E42" s="32"/>
+      <c r="F42" s="32"/>
+      <c r="G42" s="32"/>
+      <c r="H42" s="32"/>
     </row>
     <row r="43" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A43" s="2"/>
@@ -2128,12 +2176,12 @@
         <f ca="1">YEAR(DATE(Calendar3Year,Calendar3MonthOption+1,1))</f>
         <v>2019</v>
       </c>
-      <c r="C43" s="27" t="str">
+      <c r="C43" s="28" t="str">
         <f ca="1">TEXT(DATE(Calendar3Year,Calendar3MonthOption+1,1),"mmmm")</f>
         <v>July</v>
       </c>
-      <c r="D43" s="27"/>
-      <c r="E43" s="27"/>
+      <c r="D43" s="28"/>
+      <c r="E43" s="28"/>
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
@@ -2373,22 +2421,22 @@
         <f ca="1"/>
         <v>43683</v>
       </c>
-      <c r="D55" s="28" t="s">
+      <c r="D55" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="E55" s="29"/>
-      <c r="F55" s="29"/>
-      <c r="G55" s="29"/>
-      <c r="H55" s="29"/>
+      <c r="E55" s="30"/>
+      <c r="F55" s="30"/>
+      <c r="G55" s="30"/>
+      <c r="H55" s="30"/>
     </row>
     <row r="56" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B56" s="8"/>
       <c r="C56" s="8"/>
-      <c r="D56" s="31"/>
-      <c r="E56" s="31"/>
-      <c r="F56" s="31"/>
-      <c r="G56" s="31"/>
-      <c r="H56" s="31"/>
+      <c r="D56" s="32"/>
+      <c r="E56" s="32"/>
+      <c r="F56" s="32"/>
+      <c r="G56" s="32"/>
+      <c r="H56" s="32"/>
     </row>
     <row r="57" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A57" s="2"/>
@@ -2396,12 +2444,12 @@
         <f ca="1">YEAR(DATE(Calendar4Year,Calendar4MonthOption+1,1))</f>
         <v>2019</v>
       </c>
-      <c r="C57" s="27" t="str">
+      <c r="C57" s="28" t="str">
         <f ca="1">TEXT(DATE(Calendar4Year,Calendar4MonthOption+1,1),"mmmm")</f>
         <v>August</v>
       </c>
-      <c r="D57" s="27"/>
-      <c r="E57" s="27"/>
+      <c r="D57" s="28"/>
+      <c r="E57" s="28"/>
       <c r="F57" s="2"/>
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
@@ -2641,22 +2689,22 @@
         <f ca="1"/>
         <v>43711</v>
       </c>
-      <c r="D69" s="28" t="s">
+      <c r="D69" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="E69" s="29"/>
-      <c r="F69" s="29"/>
-      <c r="G69" s="29"/>
-      <c r="H69" s="29"/>
+      <c r="E69" s="30"/>
+      <c r="F69" s="30"/>
+      <c r="G69" s="30"/>
+      <c r="H69" s="30"/>
     </row>
     <row r="70" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B70" s="8"/>
       <c r="C70" s="8"/>
-      <c r="D70" s="31"/>
-      <c r="E70" s="31"/>
-      <c r="F70" s="31"/>
-      <c r="G70" s="31"/>
-      <c r="H70" s="31"/>
+      <c r="D70" s="32"/>
+      <c r="E70" s="32"/>
+      <c r="F70" s="32"/>
+      <c r="G70" s="32"/>
+      <c r="H70" s="32"/>
     </row>
     <row r="71" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A71" s="2"/>
@@ -2664,12 +2712,12 @@
         <f ca="1">YEAR(DATE(Calendar5Year,Calendar5MonthOption+1,1))</f>
         <v>2019</v>
       </c>
-      <c r="C71" s="27" t="str">
+      <c r="C71" s="28" t="str">
         <f ca="1">TEXT(DATE(Calendar5Year,Calendar5MonthOption+1,1),"mmmm")</f>
         <v>September</v>
       </c>
-      <c r="D71" s="27"/>
-      <c r="E71" s="27"/>
+      <c r="D71" s="28"/>
+      <c r="E71" s="28"/>
       <c r="F71" s="2"/>
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
@@ -2909,22 +2957,22 @@
         <f ca="1"/>
         <v>43739</v>
       </c>
-      <c r="D83" s="28" t="s">
+      <c r="D83" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="E83" s="29"/>
-      <c r="F83" s="29"/>
-      <c r="G83" s="29"/>
-      <c r="H83" s="29"/>
+      <c r="E83" s="30"/>
+      <c r="F83" s="30"/>
+      <c r="G83" s="30"/>
+      <c r="H83" s="30"/>
     </row>
     <row r="84" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B84" s="8"/>
       <c r="C84" s="8"/>
-      <c r="D84" s="31"/>
-      <c r="E84" s="31"/>
-      <c r="F84" s="31"/>
-      <c r="G84" s="31"/>
-      <c r="H84" s="31"/>
+      <c r="D84" s="32"/>
+      <c r="E84" s="32"/>
+      <c r="F84" s="32"/>
+      <c r="G84" s="32"/>
+      <c r="H84" s="32"/>
     </row>
     <row r="85" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A85" s="2"/>
@@ -2932,12 +2980,12 @@
         <f ca="1">YEAR(DATE(Calendar6Year,Calendar6MonthOption+1,1))</f>
         <v>2019</v>
       </c>
-      <c r="C85" s="27" t="str">
+      <c r="C85" s="28" t="str">
         <f ca="1">TEXT(DATE(Calendar6Year,Calendar6MonthOption+1,1),"mmmm")</f>
         <v>October</v>
       </c>
-      <c r="D85" s="27"/>
-      <c r="E85" s="27"/>
+      <c r="D85" s="28"/>
+      <c r="E85" s="28"/>
       <c r="F85" s="2"/>
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
@@ -3177,22 +3225,22 @@
         <f ca="1"/>
         <v>43774</v>
       </c>
-      <c r="D97" s="28" t="s">
+      <c r="D97" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="E97" s="29"/>
-      <c r="F97" s="29"/>
-      <c r="G97" s="29"/>
-      <c r="H97" s="29"/>
+      <c r="E97" s="30"/>
+      <c r="F97" s="30"/>
+      <c r="G97" s="30"/>
+      <c r="H97" s="30"/>
     </row>
     <row r="98" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B98" s="8"/>
       <c r="C98" s="8"/>
-      <c r="D98" s="31"/>
-      <c r="E98" s="31"/>
-      <c r="F98" s="31"/>
-      <c r="G98" s="31"/>
-      <c r="H98" s="31"/>
+      <c r="D98" s="32"/>
+      <c r="E98" s="32"/>
+      <c r="F98" s="32"/>
+      <c r="G98" s="32"/>
+      <c r="H98" s="32"/>
     </row>
     <row r="99" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A99" s="2"/>
@@ -3200,12 +3248,12 @@
         <f ca="1">YEAR(DATE(Calendar7Year,Calendar7MonthOption+1,1))</f>
         <v>2019</v>
       </c>
-      <c r="C99" s="27" t="str">
+      <c r="C99" s="28" t="str">
         <f ca="1">TEXT(DATE(Calendar7Year,Calendar7MonthOption+1,1),"mmmm")</f>
         <v>November</v>
       </c>
-      <c r="D99" s="27"/>
-      <c r="E99" s="27"/>
+      <c r="D99" s="28"/>
+      <c r="E99" s="28"/>
       <c r="F99" s="2"/>
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
@@ -3445,22 +3493,22 @@
         <f ca="1"/>
         <v>43802</v>
       </c>
-      <c r="D111" s="28" t="s">
+      <c r="D111" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="E111" s="29"/>
-      <c r="F111" s="29"/>
-      <c r="G111" s="29"/>
-      <c r="H111" s="29"/>
+      <c r="E111" s="30"/>
+      <c r="F111" s="30"/>
+      <c r="G111" s="30"/>
+      <c r="H111" s="30"/>
     </row>
     <row r="112" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B112" s="8"/>
       <c r="C112" s="8"/>
-      <c r="D112" s="31"/>
-      <c r="E112" s="31"/>
-      <c r="F112" s="31"/>
-      <c r="G112" s="31"/>
-      <c r="H112" s="31"/>
+      <c r="D112" s="32"/>
+      <c r="E112" s="32"/>
+      <c r="F112" s="32"/>
+      <c r="G112" s="32"/>
+      <c r="H112" s="32"/>
     </row>
     <row r="113" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A113" s="2"/>
@@ -3468,12 +3516,12 @@
         <f ca="1">YEAR(DATE(Calendar8Year,Calendar8MonthOption+1,1))</f>
         <v>2019</v>
       </c>
-      <c r="C113" s="27" t="str">
+      <c r="C113" s="28" t="str">
         <f ca="1">TEXT(DATE(Calendar8Year,Calendar8MonthOption+1,1),"mmmm")</f>
         <v>December</v>
       </c>
-      <c r="D113" s="27"/>
-      <c r="E113" s="27"/>
+      <c r="D113" s="28"/>
+      <c r="E113" s="28"/>
       <c r="F113" s="2"/>
       <c r="G113" s="2"/>
       <c r="H113" s="2"/>
@@ -3713,22 +3761,22 @@
         <f ca="1"/>
         <v>43830</v>
       </c>
-      <c r="D125" s="28" t="s">
+      <c r="D125" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="E125" s="29"/>
-      <c r="F125" s="29"/>
-      <c r="G125" s="29"/>
-      <c r="H125" s="29"/>
+      <c r="E125" s="30"/>
+      <c r="F125" s="30"/>
+      <c r="G125" s="30"/>
+      <c r="H125" s="30"/>
     </row>
     <row r="126" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B126" s="8"/>
       <c r="C126" s="8"/>
-      <c r="D126" s="31"/>
-      <c r="E126" s="31"/>
-      <c r="F126" s="31"/>
-      <c r="G126" s="31"/>
-      <c r="H126" s="31"/>
+      <c r="D126" s="32"/>
+      <c r="E126" s="32"/>
+      <c r="F126" s="32"/>
+      <c r="G126" s="32"/>
+      <c r="H126" s="32"/>
     </row>
     <row r="127" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A127" s="2"/>
@@ -3736,12 +3784,12 @@
         <f ca="1">YEAR(DATE(Calendar9Year,Calendar9MonthOption+1,1))</f>
         <v>2020</v>
       </c>
-      <c r="C127" s="27" t="str">
+      <c r="C127" s="28" t="str">
         <f ca="1">TEXT(DATE(Calendar9Year,Calendar9MonthOption+1,1),"mmmm")</f>
         <v>January</v>
       </c>
-      <c r="D127" s="27"/>
-      <c r="E127" s="27"/>
+      <c r="D127" s="28"/>
+      <c r="E127" s="28"/>
       <c r="F127" s="2"/>
       <c r="G127" s="2"/>
       <c r="H127" s="2"/>
@@ -3981,34 +4029,34 @@
         <f ca="1"/>
         <v>43865</v>
       </c>
-      <c r="D139" s="28" t="s">
+      <c r="D139" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="E139" s="29"/>
-      <c r="F139" s="29"/>
-      <c r="G139" s="29"/>
-      <c r="H139" s="29"/>
+      <c r="E139" s="30"/>
+      <c r="F139" s="30"/>
+      <c r="G139" s="30"/>
+      <c r="H139" s="30"/>
     </row>
     <row r="140" spans="2:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B140" s="8"/>
       <c r="C140" s="8"/>
-      <c r="D140" s="31"/>
-      <c r="E140" s="31"/>
-      <c r="F140" s="31"/>
-      <c r="G140" s="31"/>
-      <c r="H140" s="31"/>
+      <c r="D140" s="32"/>
+      <c r="E140" s="32"/>
+      <c r="F140" s="32"/>
+      <c r="G140" s="32"/>
+      <c r="H140" s="32"/>
     </row>
     <row r="141" spans="2:8" ht="54" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B141" s="1">
         <f ca="1">YEAR(DATE(Calendar10Year,Calendar10MonthOption+1,1))</f>
         <v>2020</v>
       </c>
-      <c r="C141" s="27" t="str">
+      <c r="C141" s="28" t="str">
         <f ca="1">TEXT(DATE(Calendar10Year,Calendar10MonthOption+1,1),"mmmm")</f>
         <v>February</v>
       </c>
-      <c r="D141" s="27"/>
-      <c r="E141" s="27"/>
+      <c r="D141" s="28"/>
+      <c r="E141" s="28"/>
       <c r="F141" s="2"/>
       <c r="G141" s="2"/>
       <c r="H141" s="2"/>
@@ -4247,34 +4295,34 @@
         <f ca="1"/>
         <v>43893</v>
       </c>
-      <c r="D153" s="28" t="s">
+      <c r="D153" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="E153" s="29"/>
-      <c r="F153" s="29"/>
-      <c r="G153" s="29"/>
-      <c r="H153" s="29"/>
+      <c r="E153" s="30"/>
+      <c r="F153" s="30"/>
+      <c r="G153" s="30"/>
+      <c r="H153" s="30"/>
     </row>
     <row r="154" spans="2:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B154" s="8"/>
       <c r="C154" s="8"/>
-      <c r="D154" s="31"/>
-      <c r="E154" s="31"/>
-      <c r="F154" s="31"/>
-      <c r="G154" s="31"/>
-      <c r="H154" s="31"/>
+      <c r="D154" s="32"/>
+      <c r="E154" s="32"/>
+      <c r="F154" s="32"/>
+      <c r="G154" s="32"/>
+      <c r="H154" s="32"/>
     </row>
     <row r="155" spans="2:8" ht="54" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B155" s="1">
         <f ca="1">YEAR(DATE(Calendar11Year,Calendar11MonthOption+1,1))</f>
         <v>2020</v>
       </c>
-      <c r="C155" s="27" t="str">
+      <c r="C155" s="28" t="str">
         <f ca="1">TEXT(DATE(Calendar11Year,Calendar11MonthOption+1,1),"mmmm")</f>
         <v>March</v>
       </c>
-      <c r="D155" s="27"/>
-      <c r="E155" s="27"/>
+      <c r="D155" s="28"/>
+      <c r="E155" s="28"/>
       <c r="F155" s="2"/>
       <c r="G155" s="2"/>
       <c r="H155" s="2"/>
@@ -4513,22 +4561,22 @@
         <f ca="1"/>
         <v>43921</v>
       </c>
-      <c r="D167" s="28" t="s">
+      <c r="D167" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="E167" s="29"/>
-      <c r="F167" s="29"/>
-      <c r="G167" s="29"/>
-      <c r="H167" s="29"/>
+      <c r="E167" s="30"/>
+      <c r="F167" s="30"/>
+      <c r="G167" s="30"/>
+      <c r="H167" s="30"/>
     </row>
     <row r="168" spans="2:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B168" s="8"/>
       <c r="C168" s="8"/>
-      <c r="D168" s="31"/>
-      <c r="E168" s="31"/>
-      <c r="F168" s="31"/>
-      <c r="G168" s="31"/>
-      <c r="H168" s="31"/>
+      <c r="D168" s="32"/>
+      <c r="E168" s="32"/>
+      <c r="F168" s="32"/>
+      <c r="G168" s="32"/>
+      <c r="H168" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="36">
@@ -4570,64 +4618,69 @@
     <mergeCell ref="D83:H83"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="B3:H3 B5:H5 B7:H7 B9:H9 B11:H11 B13:C13">
-    <cfRule type="expression" dxfId="12" priority="38">
+  <conditionalFormatting sqref="B3:H3 B5:H5 B9:H9 B11:H11 B13:C13">
+    <cfRule type="expression" dxfId="13" priority="39">
       <formula>MONTH(B3)&lt;&gt;Calendar1MonthOption</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:H17 B19:H19 B21:H21 B23:H23 B25:H25 B27:C27">
-    <cfRule type="expression" dxfId="11" priority="27">
+    <cfRule type="expression" dxfId="12" priority="28">
       <formula>MONTH(B17)&lt;&gt;Calendar2MonthOption</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B31:H31 B33:H33 B35:H35 B37:H37 B39:H39 B41:C41">
-    <cfRule type="expression" dxfId="10" priority="25">
+    <cfRule type="expression" dxfId="11" priority="26">
       <formula>MONTH(B31)&lt;&gt;Calendar3MonthOption</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B45:H45 B47:H47 B49:H49 B51:H51 B53:H53 B55:C55">
-    <cfRule type="expression" dxfId="9" priority="23">
+    <cfRule type="expression" dxfId="10" priority="24">
       <formula>MONTH(B45)&lt;&gt;Calendar4MonthOption</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B59:H59 B61:H61 B63:H63 B65:H65 B67:H67 B69:C69">
-    <cfRule type="expression" dxfId="8" priority="21">
+    <cfRule type="expression" dxfId="9" priority="22">
       <formula>MONTH(B59)&lt;&gt;Calendar5MonthOption</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B73:H73 B75:H75 B77:H77 B79:H79 B81:H81 B83:C83">
-    <cfRule type="expression" dxfId="7" priority="19">
+    <cfRule type="expression" dxfId="8" priority="20">
       <formula>MONTH(B73)&lt;&gt;Calendar6MonthOption</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B87:H87 B89:H89 B91:H91 B93:H93 B95:H95 B97:C97">
-    <cfRule type="expression" dxfId="6" priority="17">
+    <cfRule type="expression" dxfId="7" priority="18">
       <formula>MONTH(B87)&lt;&gt;Calendar7MonthOption</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B101:H101 B103:H103 B105:H105 B107:H107 B109:H109 B111:C111">
-    <cfRule type="expression" dxfId="5" priority="15">
+    <cfRule type="expression" dxfId="6" priority="16">
       <formula>MONTH(B101)&lt;&gt;Calendar8MonthOption</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B115:H115 B117:H117 B119:H119 B121:H121 B123:H123 B125:C125">
-    <cfRule type="expression" dxfId="4" priority="13">
+    <cfRule type="expression" dxfId="5" priority="14">
       <formula>MONTH(B115)&lt;&gt;Calendar9MonthOption</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B129:H129 B131:H131 B133:H133 B135:H135 B137:H137 B139:C139">
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>MONTH(B129)&lt;&gt;Calendar10MonthOption</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B143:H143 B145:H145 B147:H147 B149:H149 B151:H151 B153:C153">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>MONTH(B143)&lt;&gt;Calendar11MonthOption</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B157:H157 B159:H159 B161:H161 B163:H163 B165:H165 B167:C167">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>MONTH(B157)&lt;&gt;Calendar12MonthOption</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7:H7">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>MONTH(B7)&lt;&gt;Calendar1MonthOption</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations xWindow="261" yWindow="449" count="14">
@@ -4679,8 +4732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{471B5A20-71AF-48C7-9187-F7632D5EC00A}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D1"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4699,11 +4752,11 @@
         <f ca="1">YEAR(TODAY())</f>
         <v>2019</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -4808,22 +4861,26 @@
     </row>
     <row r="6" spans="1:7" ht="102.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="11"/>
-      <c r="G6" s="24"/>
+        <v>27</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="21" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
@@ -4857,19 +4914,19 @@
     </row>
     <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="9"/>
@@ -4904,22 +4961,12 @@
         <v>43583</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="60" x14ac:dyDescent="0.3">
-      <c r="A10" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>12</v>
-      </c>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
       <c r="F10" s="8"/>
       <c r="G10" s="9"/>
     </row>
@@ -4954,12 +5001,8 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>18</v>
-      </c>
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
@@ -4971,7 +5014,7 @@
     <mergeCell ref="B1:D1"/>
   </mergeCells>
   <conditionalFormatting sqref="A3:G3 A5:G5 A7:G7 A9:G9 A11:G11">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>MONTH(A3)&lt;&gt;Calendar1MonthOption</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5007,149 +5050,149 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="33"/>
+      <c r="B3" s="24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="33"/>
+      <c r="B4" s="24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="33"/>
+      <c r="B5" s="24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="33"/>
+      <c r="B6" s="24" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="33"/>
+      <c r="B7" s="24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="33"/>
+      <c r="B8" s="24" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="33"/>
+      <c r="B9" s="24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="33"/>
+      <c r="B10" s="24" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="33"/>
+      <c r="B11" s="24" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="34"/>
+      <c r="B13" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="32" t="s">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="34"/>
+      <c r="B14" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="26" t="s">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="34"/>
+      <c r="B15" s="24" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="32"/>
-      <c r="B3" s="26" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="34"/>
+      <c r="B16" s="24" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="32"/>
-      <c r="B4" s="26" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="34"/>
+      <c r="B17" s="24" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="34"/>
+      <c r="B18" s="24" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="24" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="33"/>
+      <c r="B20" s="24" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="32"/>
-      <c r="B5" s="26" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="32"/>
-      <c r="B6" s="26" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="32"/>
-      <c r="B7" s="26" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="32"/>
-      <c r="B8" s="26" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="32"/>
-      <c r="B9" s="26" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="32"/>
-      <c r="B10" s="26" t="s">
+      <c r="C20" s="24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="24" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="32"/>
-      <c r="B11" s="26" t="s">
+      <c r="B21" s="24" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="B12" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="C12" s="26" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="33"/>
-      <c r="B13" s="26" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="33"/>
-      <c r="B14" s="26" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="33"/>
-      <c r="B15" s="26" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="33"/>
-      <c r="B16" s="26" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="33"/>
-      <c r="B17" s="26" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="33"/>
-      <c r="B18" s="26" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="32" t="s">
-        <v>64</v>
-      </c>
-      <c r="B19" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="C19" s="26" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="32"/>
-      <c r="B20" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="C20" s="26" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="B21" s="26" t="s">
-        <v>68</v>
-      </c>
-      <c r="C21" s="25"/>
+      <c r="C21" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -5177,41 +5220,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="36"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="B4" s="37" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="35" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="35"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="36" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="36"/>
+      <c r="C4" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>